<commit_message>
added GMM and cleand code
</commit_message>
<xml_diff>
--- a/bycode2018.xlsx
+++ b/bycode2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabi9\Desktop\Dev\python_dev\elections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6896167E-94A9-4C08-AFAA-AC56CCC44F45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9892E1D5-D501-44EE-8997-01342C6EA369}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4108,7 +4108,7 @@
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1078" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Q6 + Q3 completed
</commit_message>
<xml_diff>
--- a/bycode2018.xlsx
+++ b/bycode2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabi9\Desktop\Dev\python_dev\elections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzmir\PycharmProjects\elections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4A9B8-870B-494D-8ABB-C3E669AFA9DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2349EF22-7E03-4D14-A563-82F8715F1AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018'!$M$1:$M$1483</definedName>
     <definedName name="IDX" localSheetId="0">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4167,8 +4167,8 @@
   <dimension ref="A1:U1483"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A556" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1489" sqref="K1489"/>
+      <pane ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18504,9 +18504,6 @@
       <c r="D293" s="1">
         <v>23</v>
       </c>
-      <c r="E293" s="1">
-        <v>234</v>
-      </c>
       <c r="F293" s="1">
         <v>9</v>
       </c>

</xml_diff>